<commit_message>
refactor: changed to konkl_type_kode in PJS_levels
</commit_message>
<xml_diff>
--- a/data-raw/PJS_levels.xlsx
+++ b/data-raw/PJS_levels.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13hopp\OneDrive - Veterinærinstituttet\R\NVIdb\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13hopp\Documents\GitHub\NVIdb\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -308,9 +308,6 @@
     <t>konkl_analyttkode</t>
   </si>
   <si>
-    <t>konkl_type</t>
-  </si>
-  <si>
     <t>sak</t>
   </si>
   <si>
@@ -333,6 +330,9 @@
   </si>
   <si>
     <t>eier_lokalitet</t>
+  </si>
+  <si>
+    <t>konkl_typekode</t>
   </si>
 </sst>
 </file>
@@ -667,8 +667,8 @@
   <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -680,25 +680,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -1052,7 +1052,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B37" s="2">
         <v>1</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="G96" s="2">
         <v>1</v>
@@ -1541,6 +1541,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004E8DCD7061C9614189F6D0F57B1C8645" ma:contentTypeVersion="9" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="d59b8845ebd1283ad3bf6a548e8d2471">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="077b9b9c-7f67-45a8-98b7-b654137cbace" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="972a228023c3d388b754ae5803fd6dc7" ns3:_="">
     <xsd:import namespace="077b9b9c-7f67-45a8-98b7-b654137cbace"/>
@@ -1718,15 +1727,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1734,6 +1734,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D016577-9F2B-4060-8113-F67317A7ACDD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4347BC88-2E0B-468E-8A95-CF71CAD2677B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1747,14 +1755,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D016577-9F2B-4060-8113-F67317A7ACDD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
feat: extended PJS_levels PJS_levels covers subundersokelse and subresultat
</commit_message>
<xml_diff>
--- a/data-raw/PJS_levels.xlsx
+++ b/data-raw/PJS_levels.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21408" windowHeight="8808"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21405" windowHeight="8805"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$G$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$I$98</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>aar</t>
   </si>
@@ -333,6 +333,45 @@
   </si>
   <si>
     <t>konkl_typekode</t>
+  </si>
+  <si>
+    <t>subundersokelse</t>
+  </si>
+  <si>
+    <t>subresultat</t>
+  </si>
+  <si>
+    <t>subundnr</t>
+  </si>
+  <si>
+    <t>subresnr</t>
+  </si>
+  <si>
+    <t>subund_avsluttet</t>
+  </si>
+  <si>
+    <t>subund_godkjent</t>
+  </si>
+  <si>
+    <t>subund_startet</t>
+  </si>
+  <si>
+    <t>subund_metodekode</t>
+  </si>
+  <si>
+    <t>subres_analyttkode</t>
+  </si>
+  <si>
+    <t>subres_kjennelsekode</t>
+  </si>
+  <si>
+    <t>subres_verdi_mengde</t>
+  </si>
+  <si>
+    <t>subres_enhetkode</t>
+  </si>
+  <si>
+    <t>subres_operator</t>
   </si>
 </sst>
 </file>
@@ -664,21 +703,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A80"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="14.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="11.5546875" style="2"/>
+    <col min="1" max="1" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="14.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="11.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -700,8 +739,14 @@
       <c r="G1" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -723,8 +768,14 @@
       <c r="G2" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -746,8 +797,14 @@
       <c r="G3" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -769,8 +826,14 @@
       <c r="G4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -789,8 +852,14 @@
       <c r="G5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>73</v>
       </c>
@@ -803,8 +872,14 @@
       <c r="F6" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>80</v>
       </c>
@@ -814,8 +889,14 @@
       <c r="F7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>84</v>
       </c>
@@ -823,8 +904,14 @@
       <c r="F8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>90</v>
       </c>
@@ -834,722 +921,806 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="4" t="s">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="4" t="s">
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="4" t="s">
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="4" t="s">
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="4" t="s">
+      <c r="C46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="4" t="s">
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="4" t="s">
+      <c r="C48" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="4" t="s">
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="4" t="s">
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="4" t="s">
+      <c r="C52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="4" t="s">
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C52" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="4" t="s">
+      <c r="C54" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C53" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="4" t="s">
+      <c r="C55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="4" t="s">
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C55" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="4" t="s">
+      <c r="C57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C56" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="4" t="s">
+      <c r="C58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C57" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="4" t="s">
+      <c r="C59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="4" t="s">
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C59" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="4" t="s">
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C60" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" s="4" t="s">
+      <c r="C62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C61" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="4" t="s">
+      <c r="C63" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C62" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="4" t="s">
+      <c r="C64" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C63" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="4" t="s">
+      <c r="C65" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C64" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="4" t="s">
+      <c r="C66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C65" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="4" t="s">
+      <c r="C67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="4" t="s">
+      <c r="C68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C67" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="4" t="s">
+      <c r="C69" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" s="4" t="s">
+      <c r="C70" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C69" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" s="4" t="s">
+      <c r="C71" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" s="4" t="s">
+      <c r="C72" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C71" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" s="4" t="s">
+      <c r="C73" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C72" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73" s="4" t="s">
+      <c r="C74" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C73" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74" s="4" t="s">
+      <c r="C75" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C74" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" s="4" t="s">
+      <c r="C76" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C75" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" s="4" t="s">
+      <c r="C77" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C76" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" s="4" t="s">
+      <c r="C78" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C77" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" s="4" t="s">
+      <c r="C79" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C78" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" s="4" t="s">
+      <c r="C80" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C79" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80" s="4" t="s">
+      <c r="C81" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D80" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="4" t="s">
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D81" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" s="4" t="s">
+      <c r="D83" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D82" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="4" t="s">
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D83" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" s="4" t="s">
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D84" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" s="4" t="s">
+      <c r="D86" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D85" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" s="4" t="s">
+      <c r="D87" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E86" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" s="4" t="s">
+      <c r="E88" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E87" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="4" t="s">
+      <c r="E89" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E88" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" s="4" t="s">
+      <c r="E90" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F89" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A90" s="4" t="s">
+      <c r="F91" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F90" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91" s="4" t="s">
+      <c r="F92" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F91" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92" s="4" t="s">
+      <c r="F93" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F92" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" s="4" t="s">
+      <c r="F94" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F93" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="4" t="s">
+      <c r="F95" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G94" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="4" t="s">
+      <c r="G96" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G95" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" s="4" t="s">
+      <c r="G97" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G96" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A97" s="4"/>
+      <c r="G98" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H99" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H100" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H101" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H102" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I103" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I104" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="I105" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I106" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I107" s="2">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G96"/>
+  <autoFilter ref="A1:I98"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004E8DCD7061C9614189F6D0F57B1C8645" ma:contentTypeVersion="9" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="d59b8845ebd1283ad3bf6a548e8d2471">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="077b9b9c-7f67-45a8-98b7-b654137cbace" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="972a228023c3d388b754ae5803fd6dc7" ns3:_="">
     <xsd:import namespace="077b9b9c-7f67-45a8-98b7-b654137cbace"/>
@@ -1727,6 +1898,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1734,14 +1914,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D016577-9F2B-4060-8113-F67317A7ACDD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4347BC88-2E0B-468E-8A95-CF71CAD2677B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1755,6 +1927,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D016577-9F2B-4060-8113-F67317A7ACDD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>